<commit_message>
final code for Get/Post Users API
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/UsersPostAPI.xlsx
+++ b/src/test/resources/exceldata/UsersPostAPI.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\star\git\DieticianAPI-Hackathon\src\test\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43270CC5-2E7D-41BD-9668-128FD39E91F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9B9AB8-7B93-4E38-AACF-C1799C57E1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E023EB60-0E3C-4029-8CA2-D4C7A83D16A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E023EB60-0E3C-4029-8CA2-D4C7A83D16A1}"/>
   </bookViews>
   <sheets>
-    <sheet name="PostUsers" sheetId="1" r:id="rId1"/>
+    <sheet name="PostUsersExistOneField" sheetId="2" r:id="rId1"/>
+    <sheet name="PostUsers" sheetId="1" r:id="rId2"/>
+    <sheet name="PostUsersUserType" sheetId="4" r:id="rId3"/>
+    <sheet name="PostUsersMissingFields" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="40">
   <si>
     <t>first_name</t>
   </si>
@@ -60,9 +63,6 @@
     <t>dietician_id</t>
   </si>
   <si>
-    <t>Neelam</t>
-  </si>
-  <si>
     <t>Snehi</t>
   </si>
   <si>
@@ -79,6 +79,75 @@
   </si>
   <si>
     <t>Patient</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>Hiranya</t>
+  </si>
+  <si>
+    <t>abcf@xyz.com</t>
+  </si>
+  <si>
+    <t>Tanvi</t>
+  </si>
+  <si>
+    <t>abcg@xyz.com</t>
+  </si>
+  <si>
+    <t>missing_field</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Allergy</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Suryakant</t>
+  </si>
+  <si>
+    <t>DT002</t>
+  </si>
+  <si>
+    <t>DT003</t>
+  </si>
+  <si>
+    <t>DT001</t>
+  </si>
+  <si>
+    <t>{"Address1":"12234","Address2":"ABC Apt 12","City":"Farmington Hills","State":"MI","Country":"USA"}</t>
+  </si>
+  <si>
+    <t>PT3647</t>
+  </si>
+  <si>
+    <t>PT6446</t>
+  </si>
+  <si>
+    <t>PT3270</t>
+  </si>
+  <si>
+    <t>PT9732</t>
+  </si>
+  <si>
+    <t>Kusharg</t>
+  </si>
+  <si>
+    <t>Anshul</t>
+  </si>
+  <si>
+    <t>abcn@xyz.com</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -123,9 +192,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -440,25 +512,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018416D0-CD08-4368-A6CA-F452658D0032}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D28179-4852-4145-A51B-24A4D125D0CC}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,37 +559,227 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
+      <c r="D2">
+        <v>1234567789</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1234567039</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1234567789</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1B0E6099-4721-446B-96B8-BA606B048C7A}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{2A71B001-FC2A-4C22-8ED9-B303CEC81AB0}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{CF97EE2B-3E10-4525-871E-4CC93041E906}"/>
+    <hyperlink ref="H3" r:id="rId4" xr:uid="{B7F072E7-0B76-4348-851B-1808A0AE1443}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{1AD8AE8F-3951-47A6-A82F-DA8C8D69A8CA}"/>
+    <hyperlink ref="H4" r:id="rId6" xr:uid="{2648BEB7-0504-4A8F-9D4A-8920C651CA5E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018416D0-CD08-4368-A6CA-F452658D0032}">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D2">
-        <v>123456789</v>
+        <v>1234567789</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -533,4 +790,254 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1388D853-2EA6-4F5E-8015-64E1939A51CA}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>1234567789</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1C2330EA-A4A5-423B-A5DF-D70757CC95A7}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{46651777-6C32-4DE7-8208-F0D6C215B32D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02DADCBE-48A3-4DC0-A2AB-73723BC94A41}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>1234567789</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1234567789</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{878E2B58-981B-436E-8A98-673100424129}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{0F58474A-3B14-4C1C-BBEA-25A4D4BECA15}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{3EB7F433-8005-4EB7-BE7B-D4FEA43E7C99}"/>
+    <hyperlink ref="H3" r:id="rId4" xr:uid="{374B39A5-CF83-4203-9345-27C7B8948E6C}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{D13EC371-9753-4507-A531-B089EE84DC67}"/>
+    <hyperlink ref="H4" r:id="rId6" xr:uid="{44196FEC-6BBC-4B94-AA1D-666F62A4AFD2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added address field in put user
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/UsersPostAPI.xlsx
+++ b/src/test/resources/exceldata/UsersPostAPI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swati\git\DieticianAPI-Hackathon\src\test\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AD21D7-C2FD-4309-90F1-049197ED54AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4C8BE8-BC6E-4628-A2F6-3C76DDC734E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E023EB60-0E3C-4029-8CA2-D4C7A83D16A1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>first_name</t>
   </si>
@@ -198,19 +198,37 @@
     <t>batman@yahoo.com</t>
   </si>
   <si>
-    <t>Milk</t>
-  </si>
-  <si>
     <t>DieticianId=DT003&amp;UserId=PT0013</t>
   </si>
   <si>
     <t>Harry</t>
   </si>
   <si>
-    <t>Potter</t>
-  </si>
-  <si>
     <t>potter@magic.com</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>{"Address1":"12234","Address2":"ABC Apt 12","City":"Farmington Hills","State":"MI","Country":"USA"}</t>
+  </si>
+  <si>
+    <t>{"Address1":"Main Rd","Address2":"Roswell","City":"Ketty","State":"TX","Country":"USA"}</t>
+  </si>
+  <si>
+    <t>{"Address1":"Main Rd","Address2":"Roswell","City":"Farmington Hills","State":"MI","Country":"USA"}</t>
+  </si>
+  <si>
+    <t>{"Address1":"Main Rd","Address2":"Apt 12","City":"Atlanta","State":"GA","Country":"USA"}</t>
+  </si>
+  <si>
+    <t>Potterr</t>
+  </si>
+  <si>
+    <t>Dek</t>
+  </si>
+  <si>
+    <t>{"Address1":"Main","Address2":"Apt 12","City":"Tampa","State":"FL","Country":"USA"}</t>
   </si>
 </sst>
 </file>
@@ -669,10 +687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1C92FC-A409-4526-A13D-2ED30B0D76FA}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,9 +701,10 @@
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="85.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -707,8 +726,11 @@
       <c r="G1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -730,8 +752,11 @@
       <c r="G2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -745,7 +770,7 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
         <v>32</v>
@@ -753,8 +778,11 @@
       <c r="G3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -776,13 +804,16 @@
       <c r="G4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>2398509030</v>
@@ -794,24 +825,27 @@
         <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C6">
         <v>345678333</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
@@ -820,7 +854,10 @@
         <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="H6" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed excel and modified schema path
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/UsersPostAPI.xlsx
+++ b/src/test/resources/exceldata/UsersPostAPI.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\star\git\DieticianAPI-Hackathon\src\test\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9B9AB8-7B93-4E38-AACF-C1799C57E1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910260C2-E85C-45A9-BC42-2D336DE7781D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E023EB60-0E3C-4029-8CA2-D4C7A83D16A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E023EB60-0E3C-4029-8CA2-D4C7A83D16A1}"/>
   </bookViews>
   <sheets>
     <sheet name="PostUsersExistOneField" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="39">
   <si>
     <t>first_name</t>
   </si>
@@ -126,34 +126,32 @@
     <t>{"Address1":"12234","Address2":"ABC Apt 12","City":"Farmington Hills","State":"MI","Country":"USA"}</t>
   </si>
   <si>
-    <t>PT3647</t>
-  </si>
-  <si>
-    <t>PT6446</t>
-  </si>
-  <si>
-    <t>PT3270</t>
-  </si>
-  <si>
-    <t>PT9732</t>
-  </si>
-  <si>
-    <t>Kusharg</t>
-  </si>
-  <si>
-    <t>Anshul</t>
-  </si>
-  <si>
-    <t>abcn@xyz.com</t>
-  </si>
-  <si>
-    <t>s</t>
+    <t>Muskan</t>
+  </si>
+  <si>
+    <t>Bauwa</t>
+  </si>
+  <si>
+    <t>abcr@xyz.com</t>
+  </si>
+  <si>
+    <t>PT685</t>
+  </si>
+  <si>
+    <t>PT9815</t>
+  </si>
+  <si>
+    <t>PT3732</t>
+  </si>
+  <si>
+    <t>PT1214</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -515,14 +513,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D28179-4852-4145-A51B-24A4D125D0CC}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -565,7 +563,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -595,7 +593,7 @@
         <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -606,7 +604,7 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>1234567039</v>
+        <v>1234567079</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
@@ -630,7 +628,7 @@
         <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -644,7 +642,7 @@
         <v>1234567789</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -665,7 +663,7 @@
         <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -683,22 +681,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018416D0-CD08-4368-A6CA-F452658D0032}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -741,7 +739,7 @@
     </row>
     <row r="2" spans="1:12" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -773,14 +771,7 @@
       <c r="K2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
+      <c r="L2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -802,7 +793,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -891,8 +882,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>